<commit_message>
Added a "Path" hedaing so the taxonomy path can be identified.
</commit_message>
<xml_diff>
--- a/src/main/resources/Alpha content master.xlsx
+++ b/src/main/resources/Alpha content master.xlsx
@@ -9472,8 +9472,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH306"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C234" workbookViewId="0">
-      <selection activeCell="F253" sqref="F253:F259"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9485,15 +9485,15 @@
     <col min="5" max="5" width="10.42578125" style="12" customWidth="1"/>
     <col min="6" max="6" width="19" style="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="12"/>
-    <col min="8" max="8" width="9.140625" style="52" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="52" hidden="1" customWidth="1"/>
-    <col min="10" max="15" width="16.28515625" style="52" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="22.140625" style="52" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="52" hidden="1" customWidth="1"/>
-    <col min="18" max="19" width="12.85546875" style="52" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="9.7109375" style="52" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="115.7109375" style="12" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="51" style="12" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="52" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="52" customWidth="1"/>
+    <col min="10" max="15" width="16.28515625" style="52" customWidth="1"/>
+    <col min="16" max="16" width="22.140625" style="52" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="52" customWidth="1"/>
+    <col min="18" max="19" width="12.85546875" style="52" customWidth="1"/>
+    <col min="20" max="21" width="9.7109375" style="52" customWidth="1"/>
+    <col min="22" max="22" width="115.7109375" style="12" customWidth="1"/>
+    <col min="23" max="23" width="94.28515625" style="12" customWidth="1"/>
     <col min="24" max="24" width="75.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="25" max="31" width="9.140625" style="12"/>
     <col min="35" max="16384" width="9.140625" style="12"/>
@@ -16710,7 +16710,7 @@
         <v>4</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C76" s="14"/>
       <c r="D76" s="14" t="s">
@@ -16735,11 +16735,11 @@
       </c>
       <c r="J76" s="52" t="str">
         <f t="shared" si="31"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="K76" s="52" t="str">
         <f t="shared" si="32"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="L76" s="52" t="str">
         <f t="shared" si="33"/>
@@ -16759,31 +16759,31 @@
       </c>
       <c r="P76" s="52" t="str">
         <f t="shared" si="37"/>
-        <v>/Economy/BalanceofPayments/timeseries/HBOP</v>
+        <v>/Economy/NationalAccounts/timeseries/HBOP</v>
       </c>
       <c r="Q76" s="52" t="str">
         <f t="shared" si="38"/>
-        <v>/Economy/BalanceofPayments//timeseries/HBOP</v>
+        <v>/Economy/NationalAccounts//timeseries/HBOP</v>
       </c>
       <c r="R76" s="52" t="str">
         <f t="shared" si="39"/>
-        <v>/Economy/BalanceofPayments/timeseries/HBOP</v>
+        <v>/Economy/NationalAccounts/timeseries/HBOP</v>
       </c>
       <c r="S76" s="52" t="str">
         <f t="shared" si="40"/>
-        <v>/Economy/BalanceofPayments/timeseries/HBOP</v>
+        <v>/Economy/NationalAccounts/timeseries/HBOP</v>
       </c>
       <c r="T76" s="52" t="str">
         <f t="shared" si="41"/>
-        <v>/economy/balanceofpayments/timeseries/hbop</v>
+        <v>/economy/nationalaccounts/timeseries/hbop</v>
       </c>
       <c r="U76" s="52" t="str">
         <f t="shared" si="42"/>
-        <v>/economy/balanceofpayments/timeseries/hbop</v>
+        <v>/economy/nationalaccounts/timeseries/hbop</v>
       </c>
       <c r="V76" s="13" t="str">
         <f t="shared" si="43"/>
-        <v>/economy/balanceofpayments/timeseries/hbop</v>
+        <v>/economy/nationalaccounts/timeseries/hbop</v>
       </c>
       <c r="W76" s="13" t="s">
         <v>1100</v>
@@ -16807,7 +16807,7 @@
         <v>4</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C77" s="14"/>
       <c r="D77" s="14" t="s">
@@ -16832,11 +16832,11 @@
       </c>
       <c r="J77" s="52" t="str">
         <f t="shared" ref="J77:J95" si="46">SUBSTITUTE(B77," ","")</f>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="K77" s="52" t="str">
         <f t="shared" ref="K77:K95" si="47">SUBSTITUTE(J77,",","")</f>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="L77" s="52" t="str">
         <f t="shared" ref="L77:L95" si="48">SUBSTITUTE(C77," ","")</f>
@@ -16856,31 +16856,31 @@
       </c>
       <c r="P77" s="52" t="str">
         <f t="shared" ref="P77:P95" si="52">CONCATENATE("/",I77,"/",K77,"/","timeseries","/",G77)</f>
-        <v>/Economy/BalanceofPayments/timeseries/IKBJ</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBJ</v>
       </c>
       <c r="Q77" s="52" t="str">
         <f t="shared" ref="Q77:Q95" si="53">CONCATENATE("/",I77,"/",K77,"/",O77,"/","timeseries","/",G77)</f>
-        <v>/Economy/BalanceofPayments//timeseries/IKBJ</v>
+        <v>/Economy/NationalAccounts//timeseries/IKBJ</v>
       </c>
       <c r="R77" s="52" t="str">
         <f t="shared" ref="R77:R108" si="54">IF(C77=0,P77,Q77)</f>
-        <v>/Economy/BalanceofPayments/timeseries/IKBJ</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBJ</v>
       </c>
       <c r="S77" s="52" t="str">
         <f t="shared" ref="S77:S95" si="55">SUBSTITUTE(R77,"-","")</f>
-        <v>/Economy/BalanceofPayments/timeseries/IKBJ</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBJ</v>
       </c>
       <c r="T77" s="52" t="str">
         <f t="shared" ref="T77:T95" si="56">LOWER(S77)</f>
-        <v>/economy/balanceofpayments/timeseries/ikbj</v>
+        <v>/economy/nationalaccounts/timeseries/ikbj</v>
       </c>
       <c r="U77" s="52" t="str">
         <f t="shared" ref="U77:U95" si="57">SUBSTITUTE(T77,"(","")</f>
-        <v>/economy/balanceofpayments/timeseries/ikbj</v>
+        <v>/economy/nationalaccounts/timeseries/ikbj</v>
       </c>
       <c r="V77" s="13" t="str">
         <f t="shared" ref="V77:V95" si="58">SUBSTITUTE(U77,")","")</f>
-        <v>/economy/balanceofpayments/timeseries/ikbj</v>
+        <v>/economy/nationalaccounts/timeseries/ikbj</v>
       </c>
       <c r="W77" s="13" t="s">
         <v>1101</v>
@@ -16904,7 +16904,7 @@
         <v>4</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C78" s="14"/>
       <c r="D78" s="14" t="s">
@@ -16929,11 +16929,11 @@
       </c>
       <c r="J78" s="52" t="str">
         <f t="shared" si="46"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="K78" s="52" t="str">
         <f t="shared" si="47"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="L78" s="52" t="str">
         <f t="shared" si="48"/>
@@ -16953,31 +16953,31 @@
       </c>
       <c r="P78" s="52" t="str">
         <f t="shared" si="52"/>
-        <v>/Economy/BalanceofPayments/timeseries/HBOJ</v>
+        <v>/Economy/NationalAccounts/timeseries/HBOJ</v>
       </c>
       <c r="Q78" s="52" t="str">
         <f t="shared" si="53"/>
-        <v>/Economy/BalanceofPayments//timeseries/HBOJ</v>
+        <v>/Economy/NationalAccounts//timeseries/HBOJ</v>
       </c>
       <c r="R78" s="52" t="str">
         <f t="shared" si="54"/>
-        <v>/Economy/BalanceofPayments/timeseries/HBOJ</v>
+        <v>/Economy/NationalAccounts/timeseries/HBOJ</v>
       </c>
       <c r="S78" s="52" t="str">
         <f t="shared" si="55"/>
-        <v>/Economy/BalanceofPayments/timeseries/HBOJ</v>
+        <v>/Economy/NationalAccounts/timeseries/HBOJ</v>
       </c>
       <c r="T78" s="52" t="str">
         <f t="shared" si="56"/>
-        <v>/economy/balanceofpayments/timeseries/hboj</v>
+        <v>/economy/nationalaccounts/timeseries/hboj</v>
       </c>
       <c r="U78" s="52" t="str">
         <f t="shared" si="57"/>
-        <v>/economy/balanceofpayments/timeseries/hboj</v>
+        <v>/economy/nationalaccounts/timeseries/hboj</v>
       </c>
       <c r="V78" s="13" t="str">
         <f t="shared" si="58"/>
-        <v>/economy/balanceofpayments/timeseries/hboj</v>
+        <v>/economy/nationalaccounts/timeseries/hboj</v>
       </c>
       <c r="W78" s="13" t="s">
         <v>1102</v>
@@ -17001,7 +17001,7 @@
         <v>4</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C79" s="14"/>
       <c r="D79" s="14" t="s">
@@ -17026,11 +17026,11 @@
       </c>
       <c r="J79" s="52" t="str">
         <f t="shared" si="46"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="K79" s="52" t="str">
         <f t="shared" si="47"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="L79" s="52" t="str">
         <f t="shared" si="48"/>
@@ -17050,31 +17050,31 @@
       </c>
       <c r="P79" s="52" t="str">
         <f t="shared" si="52"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBH</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBH</v>
       </c>
       <c r="Q79" s="52" t="str">
         <f t="shared" si="53"/>
-        <v>/Economy/BalanceofPayments//timeseries/IKBH</v>
+        <v>/Economy/NationalAccounts//timeseries/IKBH</v>
       </c>
       <c r="R79" s="52" t="str">
         <f t="shared" si="54"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBH</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBH</v>
       </c>
       <c r="S79" s="52" t="str">
         <f t="shared" si="55"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBH</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBH</v>
       </c>
       <c r="T79" s="52" t="str">
         <f t="shared" si="56"/>
-        <v>/economy/balanceofpayments/timeseries/ikbh</v>
+        <v>/economy/nationalaccounts/timeseries/ikbh</v>
       </c>
       <c r="U79" s="52" t="str">
         <f t="shared" si="57"/>
-        <v>/economy/balanceofpayments/timeseries/ikbh</v>
+        <v>/economy/nationalaccounts/timeseries/ikbh</v>
       </c>
       <c r="V79" s="13" t="str">
         <f t="shared" si="58"/>
-        <v>/economy/balanceofpayments/timeseries/ikbh</v>
+        <v>/economy/nationalaccounts/timeseries/ikbh</v>
       </c>
       <c r="W79" s="13" t="s">
         <v>1103</v>
@@ -17098,7 +17098,7 @@
         <v>4</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C80" s="14"/>
       <c r="D80" s="14" t="s">
@@ -17123,11 +17123,11 @@
       </c>
       <c r="J80" s="52" t="str">
         <f t="shared" si="46"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="K80" s="52" t="str">
         <f t="shared" si="47"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="L80" s="52" t="str">
         <f t="shared" si="48"/>
@@ -17147,31 +17147,31 @@
       </c>
       <c r="P80" s="52" t="str">
         <f t="shared" si="52"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBI</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBI</v>
       </c>
       <c r="Q80" s="52" t="str">
         <f t="shared" si="53"/>
-        <v>/Economy/BalanceofPayments//timeseries/IKBI</v>
+        <v>/Economy/NationalAccounts//timeseries/IKBI</v>
       </c>
       <c r="R80" s="52" t="str">
         <f t="shared" si="54"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBI</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBI</v>
       </c>
       <c r="S80" s="52" t="str">
         <f t="shared" si="55"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBI</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBI</v>
       </c>
       <c r="T80" s="52" t="str">
         <f t="shared" si="56"/>
-        <v>/economy/balanceofpayments/timeseries/ikbi</v>
+        <v>/economy/nationalaccounts/timeseries/ikbi</v>
       </c>
       <c r="U80" s="52" t="str">
         <f t="shared" si="57"/>
-        <v>/economy/balanceofpayments/timeseries/ikbi</v>
+        <v>/economy/nationalaccounts/timeseries/ikbi</v>
       </c>
       <c r="V80" s="13" t="str">
         <f t="shared" si="58"/>
-        <v>/economy/balanceofpayments/timeseries/ikbi</v>
+        <v>/economy/nationalaccounts/timeseries/ikbi</v>
       </c>
       <c r="W80" s="13" t="s">
         <v>1104</v>
@@ -17195,7 +17195,7 @@
         <v>4</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C81" s="14"/>
       <c r="D81" s="14" t="s">
@@ -17220,11 +17220,11 @@
       </c>
       <c r="J81" s="52" t="str">
         <f t="shared" si="46"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="K81" s="52" t="str">
         <f t="shared" si="47"/>
-        <v>BalanceofPayments</v>
+        <v>NationalAccounts</v>
       </c>
       <c r="L81" s="52" t="str">
         <f t="shared" si="48"/>
@@ -17244,31 +17244,31 @@
       </c>
       <c r="P81" s="52" t="str">
         <f t="shared" si="52"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBP</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBP</v>
       </c>
       <c r="Q81" s="52" t="str">
         <f t="shared" si="53"/>
-        <v>/Economy/BalanceofPayments//timeseries/IKBP</v>
+        <v>/Economy/NationalAccounts//timeseries/IKBP</v>
       </c>
       <c r="R81" s="52" t="str">
         <f t="shared" si="54"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBP</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBP</v>
       </c>
       <c r="S81" s="52" t="str">
         <f t="shared" si="55"/>
-        <v>/Economy/BalanceofPayments/timeseries/IKBP</v>
+        <v>/Economy/NationalAccounts/timeseries/IKBP</v>
       </c>
       <c r="T81" s="52" t="str">
         <f t="shared" si="56"/>
-        <v>/economy/balanceofpayments/timeseries/ikbp</v>
+        <v>/economy/nationalaccounts/timeseries/ikbp</v>
       </c>
       <c r="U81" s="52" t="str">
         <f t="shared" si="57"/>
-        <v>/economy/balanceofpayments/timeseries/ikbp</v>
+        <v>/economy/nationalaccounts/timeseries/ikbp</v>
       </c>
       <c r="V81" s="13" t="str">
         <f t="shared" si="58"/>
-        <v>/economy/balanceofpayments/timeseries/ikbp</v>
+        <v>/economy/nationalaccounts/timeseries/ikbp</v>
       </c>
       <c r="W81" s="13" t="s">
         <v>1105</v>

</xml_diff>